<commit_message>
Cust supp sheet with actual working for 201808
</commit_message>
<xml_diff>
--- a/Billing Request-Junos Space Support and Service Now -201808.xlsx
+++ b/Billing Request-Junos Space Support and Service Now -201808.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\pmgmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B9429FC-A5EB-4F75-9EF1-E76E7BD5C5A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0E019D-B57A-40A7-B15F-10A2365C22E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -221,7 +221,7 @@
     <t>Debayan</t>
   </si>
   <si>
-    <t>20,21,23,24,27-31</t>
+    <t xml:space="preserve">20,21, 23,24,  27-31 </t>
   </si>
 </sst>
 </file>
@@ -758,7 +758,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -893,12 +893,12 @@
         <v>43343</v>
       </c>
       <c r="G4" s="22">
-        <f>ROUND(13/21,3)</f>
-        <v>0.61899999999999999</v>
+        <f>ROUND(12/21,3)</f>
+        <v>0.57099999999999995</v>
       </c>
       <c r="H4" s="15">
         <f>D4*G4</f>
-        <v>128133</v>
+        <v>118196.99999999999</v>
       </c>
       <c r="I4" s="27">
         <v>9</v>
@@ -944,11 +944,11 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G6" s="29">
         <f>SUM(G2:G5)</f>
-        <v>3.5709999999999997</v>
+        <v>3.5229999999999997</v>
       </c>
       <c r="H6" s="7">
         <f>SUM(H2:H5)</f>
-        <v>739197</v>
+        <v>729261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>